<commit_message>
update: night point cloud filter
</commit_message>
<xml_diff>
--- a/data-result/data-measurement.xlsx
+++ b/data-result/data-measurement.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M237"/>
+  <dimension ref="A1:M277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10298,6 +10298,1646 @@
       <c r="L237" t="inlineStr"/>
       <c r="M237" t="inlineStr"/>
     </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>n15-3</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>31-81</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>n15-3_31-81_3</t>
+        </is>
+      </c>
+      <c r="E238" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F238" t="n">
+        <v>1</v>
+      </c>
+      <c r="G238" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H238" t="n">
+        <v>5310</v>
+      </c>
+      <c r="I238" t="n">
+        <v>-15.0191012456682</v>
+      </c>
+      <c r="J238" t="inlineStr"/>
+      <c r="K238" t="inlineStr"/>
+      <c r="L238" t="inlineStr"/>
+      <c r="M238" t="inlineStr"/>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>n15-3</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>31-81</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>n15-3_31-81_4</t>
+        </is>
+      </c>
+      <c r="E239" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F239" t="n">
+        <v>1</v>
+      </c>
+      <c r="G239" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H239" t="n">
+        <v>10722</v>
+      </c>
+      <c r="I239" t="n">
+        <v>-15.10511582931035</v>
+      </c>
+      <c r="J239" t="inlineStr"/>
+      <c r="K239" t="inlineStr"/>
+      <c r="L239" t="inlineStr"/>
+      <c r="M239" t="inlineStr"/>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>n15-3</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>31-81</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>n15-3_31-81_5</t>
+        </is>
+      </c>
+      <c r="E240" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F240" t="n">
+        <v>1</v>
+      </c>
+      <c r="G240" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H240" t="n">
+        <v>6805</v>
+      </c>
+      <c r="I240" t="n">
+        <v>-15.06856040476549</v>
+      </c>
+      <c r="J240" t="inlineStr"/>
+      <c r="K240" t="inlineStr"/>
+      <c r="L240" t="inlineStr"/>
+      <c r="M240" t="inlineStr"/>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>n15-3</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>31-81</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>n15-3_31-81_6</t>
+        </is>
+      </c>
+      <c r="E241" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F241" t="n">
+        <v>1</v>
+      </c>
+      <c r="G241" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H241" t="n">
+        <v>5679</v>
+      </c>
+      <c r="I241" t="n">
+        <v>-15.04382946304584</v>
+      </c>
+      <c r="J241" t="inlineStr"/>
+      <c r="K241" t="inlineStr"/>
+      <c r="L241" t="inlineStr"/>
+      <c r="M241" t="inlineStr"/>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>n15-3</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>31-81</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>n15-3_31-81_8</t>
+        </is>
+      </c>
+      <c r="E242" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F242" t="n">
+        <v>1</v>
+      </c>
+      <c r="G242" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H242" t="n">
+        <v>3847</v>
+      </c>
+      <c r="I242" t="n">
+        <v>-15.00916938878471</v>
+      </c>
+      <c r="J242" t="inlineStr"/>
+      <c r="K242" t="inlineStr"/>
+      <c r="L242" t="inlineStr"/>
+      <c r="M242" t="inlineStr"/>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>n15-5</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>31-82</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>n15-5_31-82_1</t>
+        </is>
+      </c>
+      <c r="E243" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F243" t="n">
+        <v>2</v>
+      </c>
+      <c r="G243" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H243" t="n">
+        <v>10447</v>
+      </c>
+      <c r="I243" t="n">
+        <v>-15.02340021709005</v>
+      </c>
+      <c r="J243" t="inlineStr"/>
+      <c r="K243" t="inlineStr"/>
+      <c r="L243" t="inlineStr"/>
+      <c r="M243" t="inlineStr"/>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>n15-5</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>31-82</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>n15-5_31-82_5</t>
+        </is>
+      </c>
+      <c r="E244" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F244" t="n">
+        <v>2</v>
+      </c>
+      <c r="G244" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H244" t="n">
+        <v>12931</v>
+      </c>
+      <c r="I244" t="n">
+        <v>-15.033012102153</v>
+      </c>
+      <c r="J244" t="inlineStr"/>
+      <c r="K244" t="inlineStr"/>
+      <c r="L244" t="inlineStr"/>
+      <c r="M244" t="inlineStr"/>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>n15-5</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>31-82</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>n15-5_31-82_9</t>
+        </is>
+      </c>
+      <c r="E245" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F245" t="n">
+        <v>2</v>
+      </c>
+      <c r="G245" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H245" t="n">
+        <v>3103</v>
+      </c>
+      <c r="I245" t="n">
+        <v>-15.01445987353288</v>
+      </c>
+      <c r="J245" t="inlineStr"/>
+      <c r="K245" t="inlineStr"/>
+      <c r="L245" t="inlineStr"/>
+      <c r="M245" t="inlineStr"/>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>n15-5</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>31-82</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>n15-5_31-82_4_0</t>
+        </is>
+      </c>
+      <c r="E246" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F246" t="n">
+        <v>2</v>
+      </c>
+      <c r="G246" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H246" t="n">
+        <v>5852</v>
+      </c>
+      <c r="I246" t="n">
+        <v>-15.04217628318074</v>
+      </c>
+      <c r="J246" t="inlineStr"/>
+      <c r="K246" t="inlineStr"/>
+      <c r="L246" t="inlineStr"/>
+      <c r="M246" t="inlineStr"/>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>n15-5</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>31-82</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>n15-5_31-82_7_0</t>
+        </is>
+      </c>
+      <c r="E247" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F247" t="n">
+        <v>1</v>
+      </c>
+      <c r="G247" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H247" t="n">
+        <v>4278</v>
+      </c>
+      <c r="I247" t="n">
+        <v>-14.96069443160206</v>
+      </c>
+      <c r="J247" t="inlineStr"/>
+      <c r="K247" t="inlineStr"/>
+      <c r="L247" t="inlineStr"/>
+      <c r="M247" t="inlineStr"/>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>n10-3</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>31-83</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>n10-3_31-83_2</t>
+        </is>
+      </c>
+      <c r="E248" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F248" t="n">
+        <v>1</v>
+      </c>
+      <c r="G248" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H248" t="n">
+        <v>8789</v>
+      </c>
+      <c r="I248" t="n">
+        <v>-9.994352709336807</v>
+      </c>
+      <c r="J248" t="inlineStr"/>
+      <c r="K248" t="inlineStr"/>
+      <c r="L248" t="inlineStr"/>
+      <c r="M248" t="inlineStr"/>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>n10-3</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>31-83</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>n10-3_31-83_5</t>
+        </is>
+      </c>
+      <c r="E249" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F249" t="n">
+        <v>1</v>
+      </c>
+      <c r="G249" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H249" t="n">
+        <v>8653</v>
+      </c>
+      <c r="I249" t="n">
+        <v>-9.962687887986112</v>
+      </c>
+      <c r="J249" t="inlineStr"/>
+      <c r="K249" t="inlineStr"/>
+      <c r="L249" t="inlineStr"/>
+      <c r="M249" t="inlineStr"/>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>n10-3</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>31-83</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>n10-3_31-83_6</t>
+        </is>
+      </c>
+      <c r="E250" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F250" t="n">
+        <v>1</v>
+      </c>
+      <c r="G250" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H250" t="n">
+        <v>7115</v>
+      </c>
+      <c r="I250" t="n">
+        <v>-9.988052368164062</v>
+      </c>
+      <c r="J250" t="inlineStr"/>
+      <c r="K250" t="inlineStr"/>
+      <c r="L250" t="inlineStr"/>
+      <c r="M250" t="inlineStr"/>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>n10-3</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>31-83</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>n10-3_31-83_8</t>
+        </is>
+      </c>
+      <c r="E251" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F251" t="n">
+        <v>1</v>
+      </c>
+      <c r="G251" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H251" t="n">
+        <v>7442</v>
+      </c>
+      <c r="I251" t="n">
+        <v>-9.939674058818062</v>
+      </c>
+      <c r="J251" t="inlineStr"/>
+      <c r="K251" t="inlineStr"/>
+      <c r="L251" t="inlineStr"/>
+      <c r="M251" t="inlineStr"/>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>n10-3</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>31-83</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>n10-3_31-83_11</t>
+        </is>
+      </c>
+      <c r="E252" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F252" t="n">
+        <v>1</v>
+      </c>
+      <c r="G252" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H252" t="n">
+        <v>7744</v>
+      </c>
+      <c r="I252" t="n">
+        <v>-9.928131776968831</v>
+      </c>
+      <c r="J252" t="inlineStr"/>
+      <c r="K252" t="inlineStr"/>
+      <c r="L252" t="inlineStr"/>
+      <c r="M252" t="inlineStr"/>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>n10-3</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>31-83</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>n10-3_31-83_7_0</t>
+        </is>
+      </c>
+      <c r="E253" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F253" t="n">
+        <v>1</v>
+      </c>
+      <c r="G253" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H253" t="n">
+        <v>6068</v>
+      </c>
+      <c r="I253" t="n">
+        <v>-9.948393936949454</v>
+      </c>
+      <c r="J253" t="inlineStr"/>
+      <c r="K253" t="inlineStr"/>
+      <c r="L253" t="inlineStr"/>
+      <c r="M253" t="inlineStr"/>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>n10-5</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>31-84</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>n10-5_31-84_0</t>
+        </is>
+      </c>
+      <c r="E254" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F254" t="n">
+        <v>2</v>
+      </c>
+      <c r="G254" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H254" t="n">
+        <v>5524</v>
+      </c>
+      <c r="I254" t="n">
+        <v>-10.05275608152653</v>
+      </c>
+      <c r="J254" t="inlineStr"/>
+      <c r="K254" t="inlineStr"/>
+      <c r="L254" t="inlineStr"/>
+      <c r="M254" t="inlineStr"/>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>n10-5</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>31-84</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>n10-5_31-84_2</t>
+        </is>
+      </c>
+      <c r="E255" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F255" t="n">
+        <v>2</v>
+      </c>
+      <c r="G255" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H255" t="n">
+        <v>9312</v>
+      </c>
+      <c r="I255" t="n">
+        <v>-10.0451190175959</v>
+      </c>
+      <c r="J255" t="inlineStr"/>
+      <c r="K255" t="inlineStr"/>
+      <c r="L255" t="inlineStr"/>
+      <c r="M255" t="inlineStr"/>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>n10-5</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>31-84</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>n10-5_31-84_7</t>
+        </is>
+      </c>
+      <c r="E256" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F256" t="n">
+        <v>2</v>
+      </c>
+      <c r="G256" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H256" t="n">
+        <v>14305</v>
+      </c>
+      <c r="I256" t="n">
+        <v>-10.11444208620333</v>
+      </c>
+      <c r="J256" t="inlineStr"/>
+      <c r="K256" t="inlineStr"/>
+      <c r="L256" t="inlineStr"/>
+      <c r="M256" t="inlineStr"/>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>n10-5</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>31-84</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>n10-5_31-84_8</t>
+        </is>
+      </c>
+      <c r="E257" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F257" t="n">
+        <v>2</v>
+      </c>
+      <c r="G257" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H257" t="n">
+        <v>8506</v>
+      </c>
+      <c r="I257" t="n">
+        <v>-10.09480556949652</v>
+      </c>
+      <c r="J257" t="inlineStr"/>
+      <c r="K257" t="inlineStr"/>
+      <c r="L257" t="inlineStr"/>
+      <c r="M257" t="inlineStr"/>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>n10-5</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>31-84</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>10.0</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>n10-5_31-84_10_0</t>
+        </is>
+      </c>
+      <c r="E258" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F258" t="n">
+        <v>2</v>
+      </c>
+      <c r="G258" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H258" t="n">
+        <v>8353</v>
+      </c>
+      <c r="I258" t="n">
+        <v>-10.04633404839308</v>
+      </c>
+      <c r="J258" t="inlineStr"/>
+      <c r="K258" t="inlineStr"/>
+      <c r="L258" t="inlineStr"/>
+      <c r="M258" t="inlineStr"/>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>n10-5</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>31-84</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>11.0</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>n10-5_31-84_11_0</t>
+        </is>
+      </c>
+      <c r="E259" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F259" t="n">
+        <v>2</v>
+      </c>
+      <c r="G259" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H259" t="n">
+        <v>7420</v>
+      </c>
+      <c r="I259" t="n">
+        <v>-10.05505987605088</v>
+      </c>
+      <c r="J259" t="inlineStr"/>
+      <c r="K259" t="inlineStr"/>
+      <c r="L259" t="inlineStr"/>
+      <c r="M259" t="inlineStr"/>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>n10-5</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>31-84</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>11.1</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>n10-5_31-84_11_1</t>
+        </is>
+      </c>
+      <c r="E260" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F260" t="n">
+        <v>2</v>
+      </c>
+      <c r="G260" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H260" t="n">
+        <v>9246</v>
+      </c>
+      <c r="I260" t="n">
+        <v>-10.08706795509164</v>
+      </c>
+      <c r="J260" t="inlineStr"/>
+      <c r="K260" t="inlineStr"/>
+      <c r="L260" t="inlineStr"/>
+      <c r="M260" t="inlineStr"/>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>n8-3</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>31-85</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>n8-3_31-85_1</t>
+        </is>
+      </c>
+      <c r="E261" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F261" t="n">
+        <v>2</v>
+      </c>
+      <c r="G261" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H261" t="n">
+        <v>5385</v>
+      </c>
+      <c r="I261" t="n">
+        <v>-7.930774568570478</v>
+      </c>
+      <c r="J261" t="inlineStr"/>
+      <c r="K261" t="inlineStr"/>
+      <c r="L261" t="inlineStr"/>
+      <c r="M261" t="inlineStr"/>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>n8-3</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>31-85</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>n8-3_31-85_8</t>
+        </is>
+      </c>
+      <c r="E262" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F262" t="n">
+        <v>2</v>
+      </c>
+      <c r="G262" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H262" t="n">
+        <v>15465</v>
+      </c>
+      <c r="I262" t="n">
+        <v>-8.021593506385358</v>
+      </c>
+      <c r="J262" t="inlineStr"/>
+      <c r="K262" t="inlineStr"/>
+      <c r="L262" t="inlineStr"/>
+      <c r="M262" t="inlineStr"/>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>n8-3</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>31-85</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>n8-3_31-85_9</t>
+        </is>
+      </c>
+      <c r="E263" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F263" t="n">
+        <v>2</v>
+      </c>
+      <c r="G263" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H263" t="n">
+        <v>9197</v>
+      </c>
+      <c r="I263" t="n">
+        <v>-7.974595793517354</v>
+      </c>
+      <c r="J263" t="inlineStr"/>
+      <c r="K263" t="inlineStr"/>
+      <c r="L263" t="inlineStr"/>
+      <c r="M263" t="inlineStr"/>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>n8-3</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>31-85</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>n8-3_31-85_10</t>
+        </is>
+      </c>
+      <c r="E264" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F264" t="n">
+        <v>2</v>
+      </c>
+      <c r="G264" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H264" t="n">
+        <v>8152</v>
+      </c>
+      <c r="I264" t="n">
+        <v>-7.954637771648093</v>
+      </c>
+      <c r="J264" t="inlineStr"/>
+      <c r="K264" t="inlineStr"/>
+      <c r="L264" t="inlineStr"/>
+      <c r="M264" t="inlineStr"/>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>n8-3</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>31-85</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>n8-3_31-85_7_0</t>
+        </is>
+      </c>
+      <c r="E265" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F265" t="n">
+        <v>2</v>
+      </c>
+      <c r="G265" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H265" t="n">
+        <v>10474</v>
+      </c>
+      <c r="I265" t="n">
+        <v>-7.991680181905871</v>
+      </c>
+      <c r="J265" t="inlineStr"/>
+      <c r="K265" t="inlineStr"/>
+      <c r="L265" t="inlineStr"/>
+      <c r="M265" t="inlineStr"/>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>n8-3</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>31-85</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>7.1</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>n8-3_31-85_7_1</t>
+        </is>
+      </c>
+      <c r="E266" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F266" t="n">
+        <v>2</v>
+      </c>
+      <c r="G266" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H266" t="n">
+        <v>13270</v>
+      </c>
+      <c r="I266" t="n">
+        <v>-8.012475264366786</v>
+      </c>
+      <c r="J266" t="inlineStr"/>
+      <c r="K266" t="inlineStr"/>
+      <c r="L266" t="inlineStr"/>
+      <c r="M266" t="inlineStr"/>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>n8-3</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>31-85</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>7.2</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>n8-3_31-85_7_2</t>
+        </is>
+      </c>
+      <c r="E267" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F267" t="n">
+        <v>2</v>
+      </c>
+      <c r="G267" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H267" t="n">
+        <v>6895</v>
+      </c>
+      <c r="I267" t="n">
+        <v>-7.974456587562573</v>
+      </c>
+      <c r="J267" t="inlineStr"/>
+      <c r="K267" t="inlineStr"/>
+      <c r="L267" t="inlineStr"/>
+      <c r="M267" t="inlineStr"/>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>n8-5</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>31-86</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>n8-5_31-86_0</t>
+        </is>
+      </c>
+      <c r="E268" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F268" t="n">
+        <v>1</v>
+      </c>
+      <c r="G268" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H268" t="n">
+        <v>5164</v>
+      </c>
+      <c r="I268" t="n">
+        <v>-8.004891551794712</v>
+      </c>
+      <c r="J268" t="inlineStr"/>
+      <c r="K268" t="inlineStr"/>
+      <c r="L268" t="inlineStr"/>
+      <c r="M268" t="inlineStr"/>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>n8-5</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>31-86</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>n8-5_31-86_2</t>
+        </is>
+      </c>
+      <c r="E269" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F269" t="n">
+        <v>1</v>
+      </c>
+      <c r="G269" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H269" t="n">
+        <v>10286</v>
+      </c>
+      <c r="I269" t="n">
+        <v>-7.979987757456516</v>
+      </c>
+      <c r="J269" t="inlineStr"/>
+      <c r="K269" t="inlineStr"/>
+      <c r="L269" t="inlineStr"/>
+      <c r="M269" t="inlineStr"/>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>n8-5</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>31-86</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>n8-5_31-86_5</t>
+        </is>
+      </c>
+      <c r="E270" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F270" t="n">
+        <v>1</v>
+      </c>
+      <c r="G270" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H270" t="n">
+        <v>6925</v>
+      </c>
+      <c r="I270" t="n">
+        <v>-7.931794745732919</v>
+      </c>
+      <c r="J270" t="inlineStr"/>
+      <c r="K270" t="inlineStr"/>
+      <c r="L270" t="inlineStr"/>
+      <c r="M270" t="inlineStr"/>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>n8-5</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>31-86</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>n8-5_31-86_6</t>
+        </is>
+      </c>
+      <c r="E271" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F271" t="n">
+        <v>1</v>
+      </c>
+      <c r="G271" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H271" t="n">
+        <v>11176</v>
+      </c>
+      <c r="I271" t="n">
+        <v>-7.967552575083293</v>
+      </c>
+      <c r="J271" t="inlineStr"/>
+      <c r="K271" t="inlineStr"/>
+      <c r="L271" t="inlineStr"/>
+      <c r="M271" t="inlineStr"/>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>n8-5</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>31-86</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>n8-5_31-86_10</t>
+        </is>
+      </c>
+      <c r="E272" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F272" t="n">
+        <v>1</v>
+      </c>
+      <c r="G272" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H272" t="n">
+        <v>12333</v>
+      </c>
+      <c r="I272" t="n">
+        <v>-7.912697211459546</v>
+      </c>
+      <c r="J272" t="inlineStr"/>
+      <c r="K272" t="inlineStr"/>
+      <c r="L272" t="inlineStr"/>
+      <c r="M272" t="inlineStr"/>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>n8-5</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>31-86</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>n8-5_31-86_13</t>
+        </is>
+      </c>
+      <c r="E273" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F273" t="n">
+        <v>1</v>
+      </c>
+      <c r="G273" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H273" t="n">
+        <v>7746</v>
+      </c>
+      <c r="I273" t="n">
+        <v>-7.894694196137078</v>
+      </c>
+      <c r="J273" t="inlineStr"/>
+      <c r="K273" t="inlineStr"/>
+      <c r="L273" t="inlineStr"/>
+      <c r="M273" t="inlineStr"/>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>n8-5</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>31-86</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>n8-5_31-86_14</t>
+        </is>
+      </c>
+      <c r="E274" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F274" t="n">
+        <v>1</v>
+      </c>
+      <c r="G274" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H274" t="n">
+        <v>9643</v>
+      </c>
+      <c r="I274" t="n">
+        <v>-7.902745431067421</v>
+      </c>
+      <c r="J274" t="inlineStr"/>
+      <c r="K274" t="inlineStr"/>
+      <c r="L274" t="inlineStr"/>
+      <c r="M274" t="inlineStr"/>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>n8-5</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>31-86</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>n8-5_31-86_7_0</t>
+        </is>
+      </c>
+      <c r="E275" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F275" t="n">
+        <v>1</v>
+      </c>
+      <c r="G275" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H275" t="n">
+        <v>7794</v>
+      </c>
+      <c r="I275" t="n">
+        <v>-7.946387953617993</v>
+      </c>
+      <c r="J275" t="inlineStr"/>
+      <c r="K275" t="inlineStr"/>
+      <c r="L275" t="inlineStr"/>
+      <c r="M275" t="inlineStr"/>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>n8-5</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>31-86</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>7.1</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>n8-5_31-86_7_1</t>
+        </is>
+      </c>
+      <c r="E276" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F276" t="n">
+        <v>1</v>
+      </c>
+      <c r="G276" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H276" t="n">
+        <v>6956</v>
+      </c>
+      <c r="I276" t="n">
+        <v>-7.95464317103762</v>
+      </c>
+      <c r="J276" t="inlineStr"/>
+      <c r="K276" t="inlineStr"/>
+      <c r="L276" t="inlineStr"/>
+      <c r="M276" t="inlineStr"/>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>n8-5</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>31-86</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>12.0</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>n8-5_31-86_12_0</t>
+        </is>
+      </c>
+      <c r="E277" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F277" t="n">
+        <v>1</v>
+      </c>
+      <c r="G277" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H277" t="n">
+        <v>10989</v>
+      </c>
+      <c r="I277" t="n">
+        <v>-7.892109220794155</v>
+      </c>
+      <c r="J277" t="inlineStr"/>
+      <c r="K277" t="inlineStr"/>
+      <c r="L277" t="inlineStr"/>
+      <c r="M277" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>